<commit_message>
add plot learning error of the optimal links
</commit_message>
<xml_diff>
--- a/Experiment_Results.xlsx
+++ b/Experiment_Results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xutao/PycharmProjects/Network_tomography/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{255CC1B8-6141-0342-94DF-E955649E6874}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{66F3634C-1622-514A-8B14-D39CAE074358}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45380" yWindow="980" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{364D682F-7B04-A048-A598-7CE26482F535}"/>
+    <workbookView xWindow="7800" yWindow="980" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{364D682F-7B04-A048-A598-7CE26482F535}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="fixed_monitor_percentage" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -958,19 +959,19 @@
         <v>0.67223999999999995</v>
       </c>
       <c r="C23">
-        <f t="shared" ref="C23:F23" si="0">AVERAGE(C2:C22)</f>
+        <f>AVERAGE(C2:C22)</f>
         <v>0.71034114999999998</v>
       </c>
       <c r="D23">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(D2:D22)</f>
         <v>0.70946154999999989</v>
       </c>
       <c r="E23">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(E2:E22)</f>
         <v>0.76811569999999996</v>
       </c>
       <c r="F23">
-        <f t="shared" si="0"/>
+        <f>AVERAGE(F2:F22)</f>
         <v>0.82048329999999992</v>
       </c>
     </row>
@@ -1153,19 +1154,19 @@
         <v>0.63394000000000006</v>
       </c>
       <c r="C35">
-        <f t="shared" ref="C35:F35" si="1">AVERAGE(C25:C34)</f>
+        <f>AVERAGE(C25:C34)</f>
         <v>0.60113110000000003</v>
       </c>
       <c r="D35">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(D25:D34)</f>
         <v>0.58382369999999995</v>
       </c>
       <c r="E35">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(E25:E34)</f>
         <v>0.56975730000000002</v>
       </c>
       <c r="F35">
-        <f t="shared" si="1"/>
+        <f>AVERAGE(F25:F34)</f>
         <v>0.61602299999999999</v>
       </c>
     </row>
@@ -1268,19 +1269,19 @@
         <v>0.53816249999999999</v>
       </c>
       <c r="C5" s="7">
-        <f t="shared" ref="C5:F5" si="0">(C3*20+C4*20)/40</f>
+        <f>(C3*20+C4*20)/40</f>
         <v>0.58813611499999996</v>
       </c>
       <c r="D5" s="7">
-        <f t="shared" si="0"/>
+        <f>(D3*20+D4*20)/40</f>
         <v>0.55653190499999994</v>
       </c>
       <c r="E5" s="7">
-        <f t="shared" si="0"/>
+        <f>(E3*20+E4*20)/40</f>
         <v>0.57743604999999998</v>
       </c>
       <c r="F5" s="7">
-        <f t="shared" si="0"/>
+        <f>(F3*20+F4*20)/40</f>
         <v>0.62113716500000005</v>
       </c>
     </row>
@@ -1333,19 +1334,19 @@
         <v>4.607487055</v>
       </c>
       <c r="C9" s="8">
-        <f t="shared" ref="C9:F9" si="1">(C7+C8)/2</f>
+        <f>(C7+C8)/2</f>
         <v>4.237622065</v>
       </c>
       <c r="D9" s="8">
-        <f t="shared" si="1"/>
+        <f>(D7+D8)/2</f>
         <v>4.8159205549999999</v>
       </c>
       <c r="E9" s="8">
-        <f t="shared" si="1"/>
+        <f>(E7+E8)/2</f>
         <v>5.0983303499999995</v>
       </c>
       <c r="F9" s="8">
-        <f t="shared" si="1"/>
+        <f>(F7+F8)/2</f>
         <v>5.2582709550000004</v>
       </c>
     </row>
@@ -1443,19 +1444,19 @@
         <v>0.73034250000000001</v>
       </c>
       <c r="C17" s="7">
-        <f t="shared" ref="C17:F17" si="2">AVERAGE(C13:C16)</f>
+        <f>AVERAGE(C13:C16)</f>
         <v>0.78452499999999992</v>
       </c>
       <c r="D17" s="7">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(D13:D16)</f>
         <v>0.82064333249999999</v>
       </c>
       <c r="E17" s="7">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(E13:E16)</f>
         <v>0.83891855250000003</v>
       </c>
       <c r="F17" s="7">
-        <f t="shared" si="2"/>
+        <f>AVERAGE(F13:F16)</f>
         <v>0.9028525850000001</v>
       </c>
     </row>
@@ -1544,23 +1545,23 @@
         <v>6</v>
       </c>
       <c r="B24" s="8">
-        <f t="shared" ref="B24:F24" si="3">AVERAGE(B20:B23)</f>
+        <f>AVERAGE(B20:B23)</f>
         <v>3.62672339</v>
       </c>
       <c r="C24" s="8">
-        <f t="shared" si="3"/>
+        <f>AVERAGE(C20:C23)</f>
         <v>2.700724235</v>
       </c>
       <c r="D24" s="8">
-        <f t="shared" si="3"/>
+        <f>AVERAGE(D20:D23)</f>
         <v>2.3684526075000001</v>
       </c>
       <c r="E24" s="8">
-        <f t="shared" si="3"/>
+        <f>AVERAGE(E20:E23)</f>
         <v>2.2514328324999999</v>
       </c>
       <c r="F24" s="8">
-        <f t="shared" si="3"/>
+        <f>AVERAGE(F20:F23)</f>
         <v>1.6761214575000001</v>
       </c>
     </row>
@@ -1814,7 +1815,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81467EFA-C694-4D44-8B73-934D56799AE2}">
   <dimension ref="A1:L23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>

</xml_diff>